<commit_message>
Se agregaron tablas, hasta Compra
se agregaron tablas, especificamente:
desde Orden hasta Compras
</commit_message>
<xml_diff>
--- a/Archivos no programables/DataB.xlsx
+++ b/Archivos no programables/DataB.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fjime\Documents\Erlich\Elrich\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fjime\Documents\Erlich\Erlich\Archivos no programables\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="146">
   <si>
     <t>Nombre</t>
   </si>
@@ -95,9 +95,6 @@
     <t>cantidad</t>
   </si>
   <si>
-    <t>Doctores</t>
-  </si>
-  <si>
     <t>N°JVPM</t>
   </si>
   <si>
@@ -137,9 +134,6 @@
     <t>sets</t>
   </si>
   <si>
-    <t>Pruebas</t>
-  </si>
-  <si>
     <t>subTotal</t>
   </si>
   <si>
@@ -290,12 +284,6 @@
     <t>fkHM</t>
   </si>
   <si>
-    <t>examen</t>
-  </si>
-  <si>
-    <t>idNEx</t>
-  </si>
-  <si>
     <t>Examen de orina</t>
   </si>
   <si>
@@ -465,13 +453,22 @@
   </si>
   <si>
     <t>codMedico</t>
+  </si>
+  <si>
+    <t>Medicos</t>
+  </si>
+  <si>
+    <t>relPruebaColor</t>
+  </si>
+  <si>
+    <t>idRelPC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -482,6 +479,13 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -606,7 +610,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -669,10 +673,16 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -998,7 +1008,7 @@
   <dimension ref="A1:Q54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1023,7 +1033,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="25" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="9"/>
@@ -1035,7 +1045,7 @@
       <c r="H1" s="9"/>
       <c r="I1" s="9"/>
       <c r="J1" s="9"/>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="24" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1052,7 +1062,7 @@
       <c r="D2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="23" t="str">
+      <c r="E2" s="22" t="str">
         <f>+K2</f>
         <v>nSexo</v>
       </c>
@@ -1068,8 +1078,8 @@
       </c>
       <c r="I2" s="9"/>
       <c r="J2" s="9"/>
-      <c r="K2" s="23" t="s">
-        <v>145</v>
+      <c r="K2" s="22" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -1085,7 +1095,7 @@
       <c r="J3" s="9"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="25" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="9"/>
@@ -1113,13 +1123,13 @@
         <v>codMedico</v>
       </c>
       <c r="E5" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="G5" s="8" t="s">
         <v>29</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>30</v>
       </c>
       <c r="J5" s="9"/>
     </row>
@@ -1136,7 +1146,7 @@
       <c r="J6" s="9"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="25" t="s">
         <v>17</v>
       </c>
       <c r="B7" s="9"/>
@@ -1193,7 +1203,7 @@
       <c r="J9" s="9"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="25" t="s">
         <v>6</v>
       </c>
       <c r="B10" s="9"/>
@@ -1211,7 +1221,7 @@
         <v>20</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C11" s="12" t="s">
         <v>21</v>
@@ -1221,45 +1231,57 @@
       <c r="F11" s="9"/>
       <c r="G11" s="9"/>
       <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
+      <c r="I11" s="25" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I12" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="J12" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="K12" s="12" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>23</v>
+      <c r="A13" s="24" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C14" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="6" t="s">
         <v>24</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>25</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>2</v>
       </c>
       <c r="F14" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G14" s="6" t="s">
         <v>26</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B17" s="15" t="str">
         <f>+A20</f>
@@ -1270,143 +1292,138 @@
         <v>idOrden</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E17" s="13" t="s">
         <v>7</v>
       </c>
       <c r="F17" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G17" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="G17" s="5" t="s">
+      <c r="H17" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="H17" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="I17" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="J17" s="5" t="s">
-        <v>5</v>
-      </c>
+      <c r="J17"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D20" s="15" t="s">
         <v>9</v>
       </c>
       <c r="E20" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="G20" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="F20" s="15" t="s">
+      <c r="H20" s="15" t="s">
         <v>44</v>
-      </c>
-      <c r="G20" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="H20" s="15" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D23" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B23" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C23" s="4" t="s">
+      <c r="E23" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="F23" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E23" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>52</v>
-      </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" s="22" t="s">
-        <v>65</v>
-      </c>
-      <c r="B25" s="22"/>
+      <c r="A25" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="B25" s="23"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C26" s="12" t="str">
         <f>+A11</f>
         <v>idPrueba</v>
       </c>
       <c r="D26" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F26" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="G26" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="F26" s="3" t="s">
+      <c r="H26" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="G26" s="3" t="s">
+      <c r="I26" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="H26" s="3" t="s">
+      <c r="J26" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="I26" s="3" t="s">
+      <c r="K26" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="J26" s="3" t="s">
+      <c r="L26" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="K26" s="3" t="s">
+      <c r="M26" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="L26" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="M26" s="3" t="s">
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" s="23" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="B28" s="22"/>
+      <c r="B28" s="23"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="17" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B29" s="17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C29" s="7" t="str">
         <f>+A2</f>
@@ -1425,22 +1442,22 @@
         <v>nConsist</v>
       </c>
       <c r="G29" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="H29" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="I29" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="H29" s="17" t="s">
+      <c r="J29" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="I29" s="17" t="s">
+      <c r="K29" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="J29" s="17" t="s">
+      <c r="L29" s="17" t="s">
         <v>75</v>
-      </c>
-      <c r="K29" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="L29" s="17" t="s">
-        <v>77</v>
       </c>
       <c r="M29" s="12" t="str">
         <f>+A11</f>
@@ -1449,107 +1466,98 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D31" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F31" s="22" t="s">
-        <v>81</v>
-      </c>
-      <c r="G31" s="22"/>
-      <c r="K31" s="22" t="s">
-        <v>86</v>
-      </c>
-      <c r="L31" s="22"/>
+      <c r="F31" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="G31" s="23"/>
+      <c r="K31" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="L31" s="23"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="D32" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="B32" s="21" t="str">
-        <f>+G35</f>
-        <v>idNEx</v>
-      </c>
-      <c r="D32" s="19" t="s">
-        <v>71</v>
-      </c>
       <c r="F32" s="20" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G32" s="17" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H32" s="21" t="str">
         <f>+A35</f>
         <v>idProto</v>
       </c>
       <c r="I32" s="20" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="K32" s="20" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="L32" s="17" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="M32" s="21" t="str">
         <f>+D35</f>
         <v>idMeta</v>
       </c>
       <c r="N32" s="20" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>88</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="G34"/>
+      <c r="H34"/>
       <c r="K34" s="2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="21" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B35" s="21" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D35" s="21" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E35" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="G35" s="21" t="s">
-        <v>89</v>
-      </c>
-      <c r="H35" s="21" t="s">
-        <v>9</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="G35"/>
+      <c r="H35"/>
       <c r="K35" s="19" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A37" s="22" t="s">
-        <v>90</v>
-      </c>
-      <c r="B37" s="22"/>
+      <c r="A37" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="B37" s="23"/>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" s="17" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B39" s="17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C39" s="7" t="str">
         <f>+A2</f>
@@ -1568,34 +1576,34 @@
         <v>nAspecto</v>
       </c>
       <c r="G39" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="H39" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="I39" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="J39" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="K39" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="H39" s="17" t="s">
+      <c r="L39" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="I39" s="17" t="s">
+      <c r="M39" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="J39" s="17" t="s">
+      <c r="N39" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="K39" s="17" t="s">
+      <c r="O39" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="L39" s="17" t="s">
+      <c r="P39" s="17" t="s">
         <v>100</v>
-      </c>
-      <c r="M39" s="17" t="s">
-        <v>101</v>
-      </c>
-      <c r="N39" s="17" t="s">
-        <v>102</v>
-      </c>
-      <c r="O39" s="17" t="s">
-        <v>103</v>
-      </c>
-      <c r="P39" s="17" t="s">
-        <v>104</v>
       </c>
       <c r="Q39" s="12" t="str">
         <f>+A11</f>
@@ -1604,15 +1612,15 @@
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" s="17" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B42" s="17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C42" s="7" t="str">
         <f>+C39</f>
@@ -1623,41 +1631,41 @@
         <v>codMedico</v>
       </c>
       <c r="E42" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="F42" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="G42" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="H42" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="I42" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="F42" s="17" t="s">
+      <c r="J42" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="G42" s="17" t="s">
+      <c r="K42" s="17" t="s">
         <v>109</v>
       </c>
-      <c r="H42" s="17" t="s">
+      <c r="L42" s="17" t="s">
         <v>110</v>
-      </c>
-      <c r="I42" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="J42" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="K42" s="17" t="s">
-        <v>113</v>
-      </c>
-      <c r="L42" s="17" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" s="17" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B45" s="17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C45" s="7" t="str">
         <f>+C42</f>
@@ -1668,32 +1676,32 @@
         <v>codMedico</v>
       </c>
       <c r="E45" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="F45" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="G45" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="H45" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="I45" s="17" t="s">
         <v>116</v>
-      </c>
-      <c r="F45" s="17" t="s">
-        <v>117</v>
-      </c>
-      <c r="G45" s="17" t="s">
-        <v>118</v>
-      </c>
-      <c r="H45" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="I45" s="17" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" s="17" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B48" s="17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C48" s="7" t="str">
         <f>+C45</f>
@@ -1704,35 +1712,35 @@
         <v>codMedico</v>
       </c>
       <c r="E48" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="F48" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="G48" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="H48" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="I48" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="F48" s="17" t="s">
+      <c r="J48" s="17" t="s">
         <v>123</v>
-      </c>
-      <c r="G48" s="17" t="s">
-        <v>124</v>
-      </c>
-      <c r="H48" s="17" t="s">
-        <v>125</v>
-      </c>
-      <c r="I48" s="17" t="s">
-        <v>126</v>
-      </c>
-      <c r="J48" s="17" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="17" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B51" s="17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C51" s="7" t="str">
         <f>+C48</f>
@@ -1743,66 +1751,66 @@
         <v>codMedico</v>
       </c>
       <c r="E51" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="F51" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="G51" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="H51" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="I51" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="J51" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="F51" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="G51" s="17" t="s">
+      <c r="K51" s="17" t="s">
         <v>131</v>
-      </c>
-      <c r="H51" s="17" t="s">
-        <v>132</v>
-      </c>
-      <c r="I51" s="17" t="s">
-        <v>133</v>
-      </c>
-      <c r="J51" s="17" t="s">
-        <v>134</v>
-      </c>
-      <c r="K51" s="17" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="17" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B54" s="18" t="str">
         <f>+A32</f>
         <v>nColor</v>
       </c>
       <c r="C54" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="D54" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="E54" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="F54" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="G54" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="H54" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="I54" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="D54" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="E54" s="17" t="s">
+      <c r="J54" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="F54" s="17" t="s">
+      <c r="K54" s="17" t="s">
         <v>140</v>
-      </c>
-      <c r="G54" s="17" t="s">
-        <v>116</v>
-      </c>
-      <c r="H54" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="I54" s="17" t="s">
-        <v>142</v>
-      </c>
-      <c r="J54" s="17" t="s">
-        <v>143</v>
-      </c>
-      <c r="K54" s="17" t="s">
-        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -1814,5 +1822,6 @@
     <mergeCell ref="A37:B37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>